<commit_message>
Se crea nuevo modulo para ingreso de gastos, se da mas estilo a las vistas y se genera control de accesos por roles en las demas vistas
</commit_message>
<xml_diff>
--- a/data/usuarios.xlsx
+++ b/data/usuarios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -446,9 +446,20 @@
         <v>ADMIN</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Juanita</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1234</v>
+      </c>
+      <c r="C5" t="str">
+        <v>VENDEDOR</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajustes de vistas responsive y pequeñas mejoras en filtros
</commit_message>
<xml_diff>
--- a/data/usuarios.xlsx
+++ b/data/usuarios.xlsx
@@ -415,18 +415,18 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Martha</v>
+        <v>Laura</v>
       </c>
       <c r="B2" t="str">
         <v>1234</v>
       </c>
       <c r="C2" t="str">
-        <v>ADMIN</v>
+        <v>VENDEDOR</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Laura</v>
+        <v>Juanita</v>
       </c>
       <c r="B3" t="str">
         <v>1234</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Stiven</v>
+        <v>Jorge</v>
       </c>
       <c r="B4" t="str">
         <v>1234</v>
@@ -448,13 +448,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Juanita</v>
+        <v>Stiven</v>
       </c>
       <c r="B5" t="str">
         <v>1234</v>
       </c>
       <c r="C5" t="str">
-        <v>VENDEDOR</v>
+        <v>ADMIN</v>
       </c>
     </row>
   </sheetData>

</xml_diff>